<commit_message>
lab 5 final changes
</commit_message>
<xml_diff>
--- a/lab5/Data_analysis.xlsx
+++ b/lab5/Data_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1418fc52008665ae/Documents/2XC3/lab5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{F5013A99-762D-0D40-BE14-75AC17E1624A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{404F7FBB-8EA4-4DC2-8D2D-5B066C50F825}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="13_ncr:1_{F5013A99-762D-0D40-BE14-75AC17E1624A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1182B9D-0A4B-4664-9398-8FE2B4440A75}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{013E3524-0223-374B-8896-BE28488107E4}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="4">
   <si>
     <t>Build 1</t>
   </si>
@@ -282,44 +282,8 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="power"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.59442936921287814"/>
-                  <c:y val="0.13488240193903656"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -429,44 +393,8 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="power"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.59683064987068535"/>
-                  <c:y val="1.6722708090220927E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -576,44 +504,8 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="power"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.59731081146363818"/>
-                  <c:y val="-4.1695609599930435E-3"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -1006,6 +898,859 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$51</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Build 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.172857988959901E-2"/>
+                  <c:y val="7.5759421132969712E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$52:$B$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$52:$C$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.20181200000024496</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.164057200001366</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.17124956000003466</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.18243105200001219</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.21508560419999817</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.20591247583999936</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5724-47F7-BF48-EBB0C947B86F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$51</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Build 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.12286764114641069"/>
+                  <c:y val="-9.4773325593053556E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$52:$D$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$52:$E$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.26441200000704118</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.26723780000139574</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2718208000000284</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.27746612399999943</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.29883431619999995</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.27813118823999944</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5724-47F7-BF48-EBB0C947B86F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$51</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Build 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.4956225691586203"/>
+                  <c:y val="0.43191498028664554"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$52:$F$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$52:$G$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.39905800019823745</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.67906080000739133</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.98619572000188471</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99657462600009494</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3503592629999901</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.8278964335599903</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5724-47F7-BF48-EBB0C947B86F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1617837375"/>
+        <c:axId val="1617836543"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="3"/>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:noFill/>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent4"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent4"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$E$51:$E$57</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="1">
+                        <c:v>0.26441200000704118</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.26723780000139574</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.2718208000000284</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.27746612399999943</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.29883431619999995</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.27813118823999944</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000003-5724-47F7-BF48-EBB0C947B86F}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="4"/>
+                <c:order val="4"/>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:noFill/>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent5"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent5"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$F$51:$F$57</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1000</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>10000</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>100000</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>1000000</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000004-5724-47F7-BF48-EBB0C947B86F}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1617837375"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="high"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1617836543"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1617836543"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1617837375"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1046,7 +1791,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1595,6 +2896,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>343370</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>44213</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>827852</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>188147</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86DDA734-D452-4CE6-BBC4-422CD34D882F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1912,10 +3249,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AA7228C-442C-4948-B6FF-C34F3C4EC937}">
-  <dimension ref="A3:G49"/>
+  <dimension ref="A3:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F21" zoomScale="81" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView tabSelected="1" topLeftCell="F22" zoomScale="81" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52:C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2902,8 +4239,181 @@
         <v>1827896.4335599903</v>
       </c>
     </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B51" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G51" s="4"/>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B52">
+        <f>B36</f>
+        <v>10</v>
+      </c>
+      <c r="C52">
+        <f>C44/B36</f>
+        <v>0.20181200000024496</v>
+      </c>
+      <c r="D52">
+        <f>D36</f>
+        <v>10</v>
+      </c>
+      <c r="E52">
+        <f>E44/D36</f>
+        <v>0.26441200000704118</v>
+      </c>
+      <c r="F52">
+        <f>F36</f>
+        <v>10</v>
+      </c>
+      <c r="G52">
+        <f>G44/F36</f>
+        <v>0.39905800019823745</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B53">
+        <f t="shared" ref="B53:B57" si="12">B37</f>
+        <v>100</v>
+      </c>
+      <c r="C53">
+        <f t="shared" ref="C53:C57" si="13">C45/B37</f>
+        <v>0.164057200001366</v>
+      </c>
+      <c r="D53">
+        <f t="shared" ref="D53:D57" si="14">D37</f>
+        <v>100</v>
+      </c>
+      <c r="E53">
+        <f t="shared" ref="E53:E57" si="15">E45/D37</f>
+        <v>0.26723780000139574</v>
+      </c>
+      <c r="F53">
+        <f t="shared" ref="F53:F57" si="16">F37</f>
+        <v>100</v>
+      </c>
+      <c r="G53">
+        <f t="shared" ref="G53:G57" si="17">G45/F37</f>
+        <v>0.67906080000739133</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B54">
+        <f t="shared" si="12"/>
+        <v>1000</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="13"/>
+        <v>0.17124956000003466</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="14"/>
+        <v>1000</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="15"/>
+        <v>0.2718208000000284</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="16"/>
+        <v>1000</v>
+      </c>
+      <c r="G54">
+        <f t="shared" si="17"/>
+        <v>0.98619572000188471</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B55">
+        <f t="shared" si="12"/>
+        <v>10000</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="13"/>
+        <v>0.18243105200001219</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="14"/>
+        <v>10000</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="15"/>
+        <v>0.27746612399999943</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="16"/>
+        <v>10000</v>
+      </c>
+      <c r="G55">
+        <f t="shared" si="17"/>
+        <v>0.99657462600009494</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B56">
+        <f t="shared" si="12"/>
+        <v>100000</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="13"/>
+        <v>0.21508560419999817</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="14"/>
+        <v>100000</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="15"/>
+        <v>0.29883431619999995</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="16"/>
+        <v>100000</v>
+      </c>
+      <c r="G56">
+        <f t="shared" si="17"/>
+        <v>1.3503592629999901</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B57">
+        <f t="shared" si="12"/>
+        <v>1000000</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="13"/>
+        <v>0.20591247583999936</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="14"/>
+        <v>1000000</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="15"/>
+        <v>0.27813118823999944</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="16"/>
+        <v>1000000</v>
+      </c>
+      <c r="G57">
+        <f t="shared" si="17"/>
+        <v>1.8278964335599903</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="12">
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="F51:G51"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="D43:E43"/>
     <mergeCell ref="F43:G43"/>

</xml_diff>